<commit_message>
Adding pos. mode adducts for PUAs
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adduct_ion_hierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adduct_ion_hierarchies.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/LOBSTAHS/inst/doc/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Adduct ion hierarchies" sheetId="5" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>DGCC</t>
   </si>
@@ -176,6 +181,9 @@
   </si>
   <si>
     <t>Abundance rank of adduct within lipid class</t>
+  </si>
+  <si>
+    <t>Added positive ion mode adduct ([M+H]+) for PUAs</t>
   </si>
 </sst>
 </file>
@@ -660,17 +668,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
         <v>51</v>
       </c>
@@ -687,7 +695,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -734,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -775,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -786,7 +794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -812,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -826,7 +834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -852,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -872,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -892,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -918,7 +926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -944,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -970,7 +978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1024,11 +1032,14 @@
       <c r="L14">
         <v>3</v>
       </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
       <c r="N14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1092,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1228,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1245,69 +1256,64 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42327</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42344</v>
       </c>
@@ -1337,16 +1343,22 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit updated input tables and default data
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adduct_ion_hierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adduct_ion_hierarchies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="3560" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33680" yWindow="460" windowWidth="26780" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Adduct ion hierarchies" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>DGCC</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Latest versions of all scripts and required files available at https://github.com/vanmooylipidomics/LOBSTAHS, or upon demand from Dr. Fredricks</t>
   </si>
   <si>
-    <t>Can be used to generate the file "LOBSTAHS_adduct_ion_hierarchies.csv," required for lipid-oxlipid-oxyipin database generation in the LOBSTAHS lipidomics screening pipeline</t>
-  </si>
-  <si>
     <t>To generate a .csv version of the worksheet for use with LOBSTAHS</t>
   </si>
   <si>
@@ -186,13 +183,82 @@
     <t>Added positive ion mode adduct ([M+H]+) for PUAs</t>
   </si>
   <si>
-    <t>Source data from Table 2 in Collins, J.R., B.R. Edwards, H.F. Fredricks, and B.A.S. Van Mooy, 2016, "LOBSTAHS: A Novel Lipidomics Strategy for Semi-Untargeted Discovery and Identification of Oxidative Stress Biomarkers"</t>
-  </si>
-  <si>
     <t>LPC</t>
   </si>
   <si>
     <t>Added a LPC column using same rankings as for PC (note that these have not been verified)</t>
+  </si>
+  <si>
+    <t>vGSL</t>
+  </si>
+  <si>
+    <t>sGSL</t>
+  </si>
+  <si>
+    <t>hGSL</t>
+  </si>
+  <si>
+    <t>hapGSL</t>
+  </si>
+  <si>
+    <t>PDPT</t>
+  </si>
+  <si>
+    <t>BLL</t>
+  </si>
+  <si>
+    <t>hapCER</t>
+  </si>
+  <si>
+    <t>fungalGSL</t>
+  </si>
+  <si>
+    <t>S_DGCC</t>
+  </si>
+  <si>
+    <t>plastoquinone_9</t>
+  </si>
+  <si>
+    <t>plastoquinone_9OH</t>
+  </si>
+  <si>
+    <t>plastoquinone_9OH2</t>
+  </si>
+  <si>
+    <t>ubiquinone</t>
+  </si>
+  <si>
+    <t>scytonemin</t>
+  </si>
+  <si>
+    <t>reduced_scytonemin</t>
+  </si>
+  <si>
+    <t>Source data:</t>
+  </si>
+  <si>
+    <t>Table 2 in Collins, J. R., B. R. Edwards, H. F. Fredricks, and B. A. S. Van Mooy. 2016. LOBSTAHS: An adduct-based lipidomics strategy for discovery and identification of oxidative stress biomarkers. Analytical Chemistry 88: 7154-7162; doi:10.1021/acs.analchem.6b01260</t>
+  </si>
+  <si>
+    <t>For BLL, PDPT, vGSL, sGSL, hGSL, hapGSL, and hapCER: Hunter J. E., M. J. Frada, H. F. Fredricks, A. Vardi, and B. A. S. Van Mooy. 2015. Targeted and untargeted lipidomics of Emiliania huxleyi viral infection and life cycle phases highlights molecular biomarkers of infection, susceptibility, and ploidy. Front. Mar. Sci. 2: 81; doi: 10.3389/fmars.2015.00081</t>
+  </si>
+  <si>
+    <t>The first tab of this workbook can be used to generate the file "LOBSTAHS_adduct_ion_hierarchies.csv," required for lipid-oxlipid-oxyipin database generation in the LOBSTAHS lipidomics screening pipeline</t>
+  </si>
+  <si>
+    <t>JEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added BLL, PDPT, vGSL, sGSL, hGSL, hapGSL, and hapCER (from Hunter et al., 2015; citation above) </t>
+  </si>
+  <si>
+    <t>Added S_DGCC, fungalGSLs, ubiquinones and plastoquinones</t>
+  </si>
+  <si>
+    <t>Added scytonemin and reduced scytonemin</t>
+  </si>
+  <si>
+    <t>Modifications as necessary for R function upgrades</t>
   </si>
 </sst>
 </file>
@@ -675,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,9 +753,9 @@
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -704,8 +770,23 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -737,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -754,8 +835,53 @@
       <c r="P2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -798,8 +924,38 @@
       <c r="O3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -809,8 +965,11 @@
       <c r="G4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="V4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -838,8 +997,23 @@
       <c r="K5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -853,7 +1027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -881,8 +1055,29 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -901,8 +1096,17 @@
       <c r="O8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -921,8 +1125,14 @@
       <c r="O9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>9</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -950,8 +1160,20 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>6</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -979,8 +1201,26 @@
       <c r="K11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>4</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
+      </c>
+      <c r="Y11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1008,8 +1248,23 @@
       <c r="K12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>6</v>
+      </c>
+      <c r="T12">
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <v>6</v>
+      </c>
+      <c r="X12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1037,8 +1292,29 @@
       <c r="K13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
+      <c r="X13">
+        <v>4</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1075,8 +1351,53 @@
       <c r="O14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>6</v>
+      </c>
+      <c r="AC14">
+        <v>4</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1116,8 +1437,41 @@
       <c r="P15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>7</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
+      <c r="AA15">
+        <v>6</v>
+      </c>
+      <c r="AB15">
+        <v>4</v>
+      </c>
+      <c r="AC15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1142,8 +1496,32 @@
       <c r="P16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="Z16">
+        <v>2</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1186,8 +1564,47 @@
       <c r="P17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
+      <c r="W17">
+        <v>2</v>
+      </c>
+      <c r="X17">
+        <v>2</v>
+      </c>
+      <c r="Y17">
+        <v>2</v>
+      </c>
+      <c r="Z17">
+        <v>4</v>
+      </c>
+      <c r="AA17">
+        <v>2</v>
+      </c>
+      <c r="AB17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>3</v>
+      </c>
+      <c r="AD17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1224,8 +1641,23 @@
       <c r="O18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <v>8</v>
+      </c>
+      <c r="R18">
+        <v>3</v>
+      </c>
+      <c r="T18">
+        <v>7</v>
+      </c>
+      <c r="U18">
+        <v>6</v>
+      </c>
+      <c r="AB18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1265,8 +1697,44 @@
       <c r="P19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>5</v>
+      </c>
+      <c r="S19">
+        <v>4</v>
+      </c>
+      <c r="T19">
+        <v>2</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>2</v>
+      </c>
+      <c r="W19">
+        <v>4</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+      <c r="Z19">
+        <v>3</v>
+      </c>
+      <c r="AA19">
+        <v>4</v>
+      </c>
+      <c r="AB19">
+        <v>3</v>
+      </c>
+      <c r="AC19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1276,8 +1744,38 @@
       <c r="P20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
+      </c>
+      <c r="U20">
+        <v>7</v>
+      </c>
+      <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
+        <v>5</v>
+      </c>
+      <c r="AA20">
+        <v>5</v>
+      </c>
+      <c r="AB20">
+        <v>5</v>
+      </c>
+      <c r="AC20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1287,8 +1785,11 @@
       <c r="P21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="AB21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1298,10 +1799,34 @@
       <c r="P22">
         <v>3</v>
       </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>7</v>
+      </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+      <c r="W22">
+        <v>3</v>
+      </c>
+      <c r="X22">
+        <v>3</v>
+      </c>
+      <c r="Y22">
+        <v>3</v>
+      </c>
+      <c r="AB22">
+        <v>7</v>
+      </c>
+      <c r="AC22">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:P1"/>
+    <mergeCell ref="C1:AE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1310,16 +1835,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1329,67 +1854,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>46</v>
+      <c r="B3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
+      <c r="A4" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
+      <c r="A12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>42327</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>42344</v>
+        <v>42327</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1397,10 +1919,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>42403</v>
+        <v>42344</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1408,12 +1930,67 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>42607</v>
       </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>42624</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>42709</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>42719</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>42758</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>